<commit_message>
Improve app to work with Tables UI tests
</commit_message>
<xml_diff>
--- a/app/config/tables/testRun/forms/testRun/testRun.xlsx
+++ b/app/config/tables/testRun/forms/testRun/testRun.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="6140" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="25280" yWindow="5960" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>type</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>testId</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>Database Used</t>
+  </si>
+  <si>
+    <t>services</t>
+  </si>
+  <si>
+    <t>Services Used</t>
+  </si>
+  <si>
+    <t>all_in_one</t>
+  </si>
+  <si>
+    <t>All In One APK Used</t>
   </si>
 </sst>
 </file>
@@ -522,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -658,45 +676,84 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="4"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="6"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>